<commit_message>
RUV_OECD space in sector 4-5 correction
</commit_message>
<xml_diff>
--- a/exercise_OECD_data/0-Raw_Data/sectors_WIOD_SEA_final.xlsx
+++ b/exercise_OECD_data/0-Raw_Data/sectors_WIOD_SEA_final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mabad\OneDrive\Documentos\GitHub\RUV\exercise_OECD_data\0-Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CED39C-C1AC-4F15-B0E6-7D7033470BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C0799D-0413-4DEC-8F87-81D13F0CA507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14592" xr2:uid="{D40FFF6D-7836-43BE-9EE9-20846187756A}"/>
   </bookViews>
@@ -102,15 +102,9 @@
     <t>C18</t>
   </si>
   <si>
-    <t xml:space="preserve">Manufacture of coke and refined petroleum products </t>
-  </si>
-  <si>
     <t>C19</t>
   </si>
   <si>
-    <t xml:space="preserve">Manufacture of chemicals and chemical products </t>
-  </si>
-  <si>
     <t>C20</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>E36</t>
   </si>
   <si>
-    <t xml:space="preserve">Sewerage; waste collection, treatment and disposal activities; materials recovery; remediation activities and other waste management services </t>
-  </si>
-  <si>
     <t>E37-E39</t>
   </si>
   <si>
@@ -379,6 +370,15 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>Manufacture of coke and refined petroleum products</t>
+  </si>
+  <si>
+    <t>Manufacture of chemicals and chemical products</t>
+  </si>
+  <si>
+    <t>Sewerage; waste collection, treatment and disposal activities; materials recovery; remediation activities and other waste management services</t>
   </si>
 </sst>
 </file>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{628AA1D4-28A5-4310-B50B-6D4BA3A832BB}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -893,10 +893,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -915,10 +915,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -937,10 +937,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -948,10 +948,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -959,10 +959,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -970,10 +970,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20">
         <v>9</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>11</v>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>11</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23">
         <v>12</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>13</v>
@@ -1047,26 +1047,26 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C27">
         <v>13</v>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>13</v>
@@ -1085,10 +1085,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29">
         <v>13</v>
@@ -1096,10 +1096,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C30">
         <v>13</v>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C31" s="1">
         <v>13</v>
@@ -1118,10 +1118,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1">
         <v>13</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1">
         <v>13</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1">
         <v>13</v>
@@ -1151,10 +1151,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C35" s="1">
         <v>13</v>
@@ -1162,10 +1162,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C36" s="1">
         <v>13</v>
@@ -1173,10 +1173,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1">
         <v>13</v>
@@ -1184,10 +1184,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1">
         <v>13</v>
@@ -1195,10 +1195,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C39" s="1">
         <v>13</v>
@@ -1206,10 +1206,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" s="1">
         <v>13</v>
@@ -1217,10 +1217,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1">
         <v>13</v>
@@ -1228,10 +1228,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1">
         <v>13</v>
@@ -1239,10 +1239,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1">
         <v>13</v>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1">
         <v>13</v>
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C45" s="1">
         <v>13</v>
@@ -1272,10 +1272,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C46" s="1">
         <v>13</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C47" s="1">
         <v>13</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1">
         <v>13</v>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C49" s="1">
         <v>13</v>
@@ -1316,10 +1316,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C50" s="1">
         <v>13</v>
@@ -1327,10 +1327,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C51" s="1">
         <v>13</v>
@@ -1338,19 +1338,19 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C53" s="1">
         <v>13</v>
@@ -1358,10 +1358,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C54" s="1">
         <v>13</v>
@@ -1369,10 +1369,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C55" s="1">
         <v>13</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C56" s="1">
         <v>13</v>
@@ -1391,10 +1391,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C57" s="1"/>
     </row>

</xml_diff>